<commit_message>
Se agrega importacion por XML y Email (facturas@etaxcr.com) de facturas recibidas. Se crea pantalla de aceptacion de facturas
</commit_message>
<xml_diff>
--- a/public/assets/files/PlantillaLineasFacturaEmitida.xlsx
+++ b/public/assets/files/PlantillaLineasFacturaEmitida.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alf-g\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E29008DC-68BE-4B28-A19F-941136AA8CC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921AB2DA-EC3A-4B0B-A1C2-A60003156867}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1467" yWindow="1467" windowWidth="19200" windowHeight="10073" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PaginaDetalle" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
-    <t>IdTipoDocumento</t>
-  </si>
-  <si>
     <t>ConsecutivoComprobante</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>MontoDescuento</t>
   </si>
   <si>
-    <t>CodigoImpuesto</t>
-  </si>
-  <si>
     <t>TotalLinea</t>
   </si>
   <si>
@@ -113,6 +107,12 @@
   </si>
   <si>
     <t>EJCodigo</t>
+  </si>
+  <si>
+    <t>TipoDocumento</t>
+  </si>
+  <si>
+    <t>CodigoEtax</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
     <sortCondition ref="B1:B2"/>
   </sortState>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="IdTipoDocumento" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TipoDocumento" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ConsecutivoComprobante" dataDxfId="19"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="IdMoneda" dataDxfId="18"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TipoCambio" dataDxfId="17"/>
@@ -264,7 +264,7 @@
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="PrecioUnitario" dataDxfId="6"/>
     <tableColumn id="27" xr3:uid="{F2DD17B1-2A7F-44F4-9597-E795BCF624ED}" name="SubtotalLinea" dataDxfId="5"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MontoDescuento" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="CodigoImpuesto" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="CodigoEtax" dataDxfId="3"/>
     <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="MontoIVA" dataDxfId="2"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TotalLinea" dataDxfId="1"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="TotalDocumento" dataDxfId="0"/>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -584,78 +584,79 @@
     <col min="13" max="13" width="21.703125" customWidth="1"/>
     <col min="16" max="16" width="9.05859375" customWidth="1"/>
     <col min="18" max="18" width="10.234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.64453125" customWidth="1"/>
     <col min="21" max="21" width="12.17578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -663,43 +664,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>28</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
       </c>
       <c r="O2">
         <v>1</v>

</xml_diff>

<commit_message>
Nuevo reporte y otros cambios
</commit_message>
<xml_diff>
--- a/public/assets/files/PlantillaLineasFacturaEmitida.xlsx
+++ b/public/assets/files/PlantillaLineasFacturaEmitida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06826101-968D-4EDE-A773-343E3C966E58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E156A4C-1EEF-4F4D-93A2-B65209B97AE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PaginaDetalle" sheetId="1" r:id="rId1"/>
@@ -1572,6 +1572,16 @@
           <t xml:space="preserve">
 </t>
         </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
       </text>
     </comment>
     <comment ref="U2" authorId="0" shapeId="0" xr:uid="{113E9FA5-BE92-1D49-B526-F17CEC02F5F4}">
@@ -1841,25 +1851,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>130</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Ventas de bienes y servicios con límites sobrepasados 13% con derecho a crédito 
+          <t xml:space="preserve">130 - Ventas de bienes y servicios con límites sobrepasados 13% con derecho a crédito 
 </t>
         </r>
         <r>
@@ -2029,25 +2021,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">250 - </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ventas a sujetos exentos</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
+          <t xml:space="preserve">250 - Ventas a sujetos exentos 
 </t>
         </r>
         <r>
@@ -2129,27 +2103,9 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Verifique este dato </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>y si lo desea, puede sobreescribir el cálculo automático digitando manualmente otro número.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Verifique este dato y si lo desea, puede sobreescribir el cálculo automático digitando manualmente otro número.
 </t>
         </r>
         <r>
@@ -2178,7 +2134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>ConsecutivoComprobante</t>
   </si>
@@ -2334,21 +2290,9 @@
     <t>Indique el detalle de producto definido en la línea de la factura.</t>
   </si>
   <si>
-    <t>Elija la unidad de medición detallada en la línea de la factura.</t>
-  </si>
-  <si>
     <t>CodigoIVAEtax</t>
   </si>
   <si>
-    <t>Cálculo automático: monto de IVA correspondiente al subtotal de línea</t>
-  </si>
-  <si>
-    <t>Cálculo automático: subtotal de la línea.</t>
-  </si>
-  <si>
-    <t>Cálculo automático: Total de línea</t>
-  </si>
-  <si>
     <t>Indique el monto total de la factura</t>
   </si>
   <si>
@@ -2364,23 +2308,66 @@
     <t>Unid</t>
   </si>
   <si>
-    <t>XXXXXXXXX</t>
+    <r>
+      <t xml:space="preserve">Subtotal de la línea. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Este es un cálculo automático. Verifique el dato en su factura y cambiélo manualmente en caso de ser necesario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Monto de IVA correspondiente al subtotal de línea. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Este es un cálculo automático. Verifique el dato en su factura y cambiélo manualmente en caso de ser necesario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total de línea. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Este es un cálculo automático. Verifique el dato en su factura y cambiélo manualmente en caso de ser necesario.</t>
+    </r>
+  </si>
+  <si>
+    <t>Indique la unidad de medición detallada en la línea de la factura.</t>
   </si>
   <si>
     <t>CorreoReceptor</t>
   </si>
   <si>
-    <t>Indique el correo electrónico del receptor</t>
-  </si>
-  <si>
-    <t>ejemplo@dominio.com</t>
+    <t>Indique el correo electrónico de su cliente</t>
+  </si>
+  <si>
+    <t>ejemplo@etaxcr.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2427,6 +2414,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -2452,7 +2445,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2485,7 +2478,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2505,6 +2498,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2601,7 +2595,7 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NombreCliente" dataDxfId="15"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TipoIdentificacion" dataDxfId="14"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IdentificacionReceptor" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{55D9B701-FABB-457C-AA96-585300CCF04D}" name="CorreoReceptor" dataCellStyle="Hyperlink"/>
+    <tableColumn id="14" xr3:uid="{9EE5C575-439A-401D-844A-0CF2ADD0E6CE}" name="CorreoReceptor" dataCellStyle="Hyperlink"/>
     <tableColumn id="25" xr3:uid="{416EB538-A7AD-494E-B673-8B653787523A}" name="CondicionVenta"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="MetodoPago" dataDxfId="12"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NumeroLinea" dataDxfId="11"/>
@@ -2615,7 +2609,9 @@
     </tableColumn>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MontoDescuento" dataDxfId="4"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="CodigoIVAEtax" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="MontoIVA" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="MontoIVA" dataDxfId="2">
+      <calculatedColumnFormula>S4*IF(U4=103,13%,IF(U4=101,1%,IF(U4=102,2%,IF(U4=104,4%,IF(U4=114,4%,IF(U4=118,8%,IF(U4=121,1%,IF(U4=122,2%,IF(U4=123,13%,IF(U4=124,4%,IF(U4=130,13%,IF(U4=140,13%,0))))))))))))</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TotalLinea" dataDxfId="1">
       <calculatedColumnFormula>S4-T4+V4</calculatedColumnFormula>
     </tableColumn>
@@ -2924,11 +2920,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="20.77734375" style="9" customWidth="1"/>
@@ -2936,14 +2932,17 @@
     <col min="4" max="4" width="20.77734375" customWidth="1"/>
     <col min="5" max="6" width="15.77734375" customWidth="1"/>
     <col min="7" max="7" width="20.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
     <col min="9" max="10" width="20.77734375" customWidth="1"/>
     <col min="11" max="18" width="15.77734375" customWidth="1"/>
-    <col min="19" max="19" width="15.77734375" style="1" customWidth="1"/>
-    <col min="20" max="24" width="15.77734375" customWidth="1"/>
+    <col min="19" max="19" width="25.77734375" style="1" customWidth="1"/>
+    <col min="20" max="21" width="15.77734375" customWidth="1"/>
+    <col min="22" max="22" width="28.33203125" customWidth="1"/>
+    <col min="23" max="23" width="25.77734375" customWidth="1"/>
+    <col min="24" max="24" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="64.95" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>40</v>
       </c>
@@ -2971,7 +2970,7 @@
       <c r="W1" s="16"/>
       <c r="X1" s="16"/>
     </row>
-    <row r="2" spans="1:24" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="4" customFormat="1" ht="49.95" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -3000,7 +2999,7 @@
         <v>36</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>37</v>
@@ -3021,31 +3020,31 @@
         <v>43</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="R2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="X2" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -3074,7 +3073,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>12</v>
@@ -3107,7 +3106,7 @@
         <v>9</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>16</v>
@@ -3119,7 +3118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3144,11 +3143,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>55</v>
+      <c r="I4" s="8">
+        <v>114170404</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -3169,7 +3168,7 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="R4">
         <v>1000</v>
@@ -3185,6 +3184,7 @@
         <v>103</v>
       </c>
       <c r="V4">
+        <f t="shared" ref="V4" si="0">S4*IF(U4=103,13%,IF(U4=101,1%,IF(U4=102,2%,IF(U4=104,4%,IF(U4=114,4%,IF(U4=118,8%,IF(U4=121,1%,IF(U4=122,2%,IF(U4=123,13%,IF(U4=124,4%,IF(U4=130,13%,IF(U4=140,13%,0))))))))))))</f>
         <v>130</v>
       </c>
       <c r="W4" s="1">
@@ -3199,7 +3199,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:X1"/>
   </mergeCells>
-  <dataValidations count="7">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4" xr:uid="{AC2F3921-FC38-9548-AC79-E72BE78E27E2}">
       <formula1>"1, 2, 3, 4, 5, 6, 7, 8, 99"</formula1>
     </dataValidation>
@@ -3218,15 +3218,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4" xr:uid="{A99C6C29-6598-9B48-AAFF-A836F2595B96}">
       <formula1>"101, 102, 103, 104,114,118,121,122,123,124,130,140,150,160,200,201,240,245,250,260"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4" xr:uid="{96268742-5CD7-E94B-8959-07CAA6371FA5}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{0DB384F6-F56C-43A3-B64C-07504588F0BE}"/>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{FDAD6757-4301-41CC-A48A-D6BB3898384E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="B4" numberStoredAsText="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
     <tablePart r:id="rId4"/>

</xml_diff>

<commit_message>
Add: Clasificacion de ventas por linea, codigos custodios, fix Excel con cedula contribuyente
</commit_message>
<xml_diff>
--- a/public/assets/files/PlantillaLineasFacturaEmitida.xlsx
+++ b/public/assets/files/PlantillaLineasFacturaEmitida.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99487ABC-3934-4F3A-B46A-E08B1EE51BFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C85C17-AB7B-4BDA-B509-40DF800FE7B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{EAE1ADED-6078-F04D-B8B1-7838C9C1AC4D}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{BDDC2A1D-A25C-46A9-A741-ACC39AE024A0}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tipos de divisas:</t>
+          <t>Códigos de tipo de documento</t>
         </r>
         <r>
           <rPr>
@@ -176,31 +176,91 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">CRC - colón costarricense
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">USD - dólar estadounidense
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>EUR - euro</t>
+          <t xml:space="preserve">1 - Factura electrónica
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 - Nota de débito electrónica
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 - Nota de crédito electrónica
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4 - Tiquete electrónico
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 - Nota de despacho
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">6- Contrato
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">7 - Procedimiento
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">8 - Comprobante emitido en contingencia
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>99 - Otros</t>
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{98A2A71A-E148-A645-A8E1-C7DCC8982F54}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{EAE1ADED-6078-F04D-B8B1-7838C9C1AC4D}">
       <text>
         <r>
           <rPr>
@@ -210,7 +270,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sobre el tipo de cambio:</t>
+          <t>Tipos de divisas:</t>
         </r>
         <r>
           <rPr>
@@ -229,21 +289,31 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Si la venta fue en CRC, se debe digitar 1.</t>
+          <t xml:space="preserve">CRC - colón costarricense
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">USD - dólar estadounidense
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>EUR - euro</t>
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{9B8061AE-5263-7F40-984B-791F48BE633F}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{98A2A71A-E148-A645-A8E1-C7DCC8982F54}">
       <text>
         <r>
           <rPr>
@@ -253,7 +323,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código de cliente:</t>
+          <t>Sobre el tipo de cambio:</t>
         </r>
         <r>
           <rPr>
@@ -270,17 +340,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">El código de cliente es un código definido por usted que se utiliza para ordenar  sus clientes en eTax.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -290,13 +350,13 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t>Digite el código previamente creado en eTax para clientes existentes, o bien, defina un código nuevo para clientes nuevos.</t>
+            <family val="2"/>
+          </rPr>
+          <t>Si la venta fue en CRC, se debe digitar 1.</t>
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{AF6609EE-8FE5-5849-93A5-E0A19B8B98BF}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{9B8061AE-5263-7F40-984B-791F48BE633F}">
       <text>
         <r>
           <rPr>
@@ -306,7 +366,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código de identificación:</t>
+          <t>Código de cliente:</t>
         </r>
         <r>
           <rPr>
@@ -323,63 +383,33 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">1 - Cédula física
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">2 - Cédula jurídica
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">3 - DIMEX
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">4 - NITE
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">5 - Extranjero
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>6 - Otro</t>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">El código de cliente es un código definido por usted que se utiliza para ordenar  sus clientes en eTax.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t>Digite el código previamente creado en eTax para clientes existentes, o bien, defina un código nuevo para clientes nuevos.</t>
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{A1D71C11-1F3F-5A41-83E2-F04BDA5B15F3}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{AF6609EE-8FE5-5849-93A5-E0A19B8B98BF}">
       <text>
         <r>
           <rPr>
@@ -389,7 +419,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sobre el número de identificación:</t>
+          <t>Código de identificación:</t>
         </r>
         <r>
           <rPr>
@@ -408,41 +438,61 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Escriba el número sin guiones. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>En el caso de cédulas físicas, el número debe contener 9 dígitos. Si el número de cédula es más corto, complete con ceros.</t>
+          <t xml:space="preserve">1 - Cédula física
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 - Cédula jurídica
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 - DIMEX
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4 - NITE
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 - Extranjero
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>6 - Otro</t>
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{283C71F2-2D3A-C24F-9004-6BCBCCE00BBD}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{A1D71C11-1F3F-5A41-83E2-F04BDA5B15F3}">
       <text>
         <r>
           <rPr>
@@ -452,7 +502,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Códigos de condición de venta:</t>
+          <t>Sobre el número de identificación:</t>
         </r>
         <r>
           <rPr>
@@ -471,71 +521,41 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">1 - Contado
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">2 - Crédito
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">3 - Consignación
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">4 - Apartado
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">5 - Arrendamiento con opción de compra
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">6 - Arrendamiento en función financiera
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>99 - Otros</t>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Escriba el número sin guiones. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>En el caso de cédulas físicas, el número debe contener 9 dígitos. Si el número de cédula es más corto, complete con ceros.</t>
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{B340FF8E-F337-3A45-B79B-E64EB08A6290}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{283C71F2-2D3A-C24F-9004-6BCBCCE00BBD}">
       <text>
         <r>
           <rPr>
@@ -545,7 +565,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Códigos de método de pago:</t>
+          <t>Códigos de condición de venta:</t>
         </r>
         <r>
           <rPr>
@@ -564,47 +584,57 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">1 - Efectivo
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">2 - Tarjeta
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">3 - Cheque
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">4 - Transferencia - depósito bancario
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">5 - Recaudado por terceros
+          <t xml:space="preserve">1 - Contado
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 - Crédito
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 - Consignación
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4 - Apartado
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 - Arrendamiento con opción de compra
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">6 - Arrendamiento en función financiera
 </t>
         </r>
         <r>
@@ -618,7 +648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{1470636F-4ECF-9B44-BFEB-D0693805F864}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{B340FF8E-F337-3A45-B79B-E64EB08A6290}">
       <text>
         <r>
           <rPr>
@@ -628,7 +658,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código de producto:</t>
+          <t>Códigos de método de pago:</t>
         </r>
         <r>
           <rPr>
@@ -645,44 +675,63 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">El código de producto es un código definido por usted que se utiliza para ordenar  sus productos en eTax.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Digite el código previamente creado en eTax para productos existentes, o bien, defina un código nuevo para productos nuevos.
-</t>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 - Efectivo
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 - Tarjeta
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 - Cheque
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">4 - Transferencia - depósito bancario
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 - Recaudado por terceros
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>99 - Otros</t>
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{F583B32F-3226-104C-8032-58313B21AECE}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{1470636F-4ECF-9B44-BFEB-D0693805F864}">
       <text>
         <r>
           <rPr>
@@ -692,7 +741,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Unidades de medida:</t>
+          <t>Código de producto:</t>
         </r>
         <r>
           <rPr>
@@ -711,866 +760,6 @@
             <rFont val="Tahoma"/>
             <family val="34"/>
           </rPr>
-          <t xml:space="preserve">Unidad - Unid
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Servicios Profesionales - Sp
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">1 por metro - 1/m
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Alquiler de uso comercial - Alc
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Alquiler de uso habitacional - Al
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Ampere - A
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">ampere por metro - A/m
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">ampere por metro cuadrado - A/m²
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Becquerel - Bq
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">bel - B
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Candela - cd
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">candela por metro cuadrado - cd/m²
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">centímetro - cm
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Comisiones - Cm
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">coulomb - C
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">coulomb por kilogramo - C/kg
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">coulomb por metro cuadrado - C/m²
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">coulomb por metro cúbico - C/m³
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">día - d
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">electronvolt - eV
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">estereorradión - sr
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">farad - F
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">farad por metro - F/m
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Galán - Gal
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">grado - deg
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">grado Celsius - C
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Gramo - g
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">gray - Gy
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">gray por segundo - Gy/s
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">henry - H
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">henry por metro - H/m
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">hertz - Hz
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">hora - h
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Intereses - I
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Joule - J
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">joule por kelvin - J/K
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">joule por kilogramo - J/kg
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">joule por metro cúbico - J/m³
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">joule por mol - J/mol
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">katal - kat
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">katal por metro cúbico - kat/m³
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Kelvin - K
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Kilogramo - kg
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">kilogramo por metro cúbico - kg/m³
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Kilometro - Km
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">kilovatios - Kw
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">litro - L
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">lumen - lm
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">lux - lx
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Metro - m
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">metro cuadrado - m²
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">metro cúbico - m³
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">metro por segundo - m/s
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">mililitro - mL
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Milímetro - mm
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">minuto - min
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Mol - mol
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">mol por metro cúbico - mol/m³
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">neper - Np
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">newton - N
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">newton por metro - N/m
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Onzas - Oz
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Otro tipo de servicio - Os
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">pascal - Pa
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">pascal segundo - Pa s
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">pulgada - ln
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">radión - rad
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">radión por segundo - rad/s
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Se debe indicar la descripción de la medida a utilizar - Otros
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">segundo - s
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Servicios personales - Spe
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Servicios técnicos - St
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">siemens - S
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">sievert - Sv
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">tesla - T
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">tonelada - t
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">unidad astronómica - ua
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">unidad de masa atómica unificada - u
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">uno (indice de refracción) - 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">volt - V
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">volt por metro - V/m
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">Watt - W
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">watt por estereorradión - W/sr
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">watt por metro cuadrado - W/m²
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">watt por metro kevin - W/(mxK)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="34"/>
-          </rPr>
-          <t xml:space="preserve">weber - Wb
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">
 </t>
         </r>
@@ -1578,15 +767,939 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">El código de producto es un código definido por usted que se utiliza para ordenar  sus productos en eTax.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Digite el código previamente creado en eTax para productos existentes, o bien, defina un código nuevo para productos nuevos.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{113E9FA5-BE92-1D49-B526-F17CEC02F5F4}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{F583B32F-3226-104C-8032-58313B21AECE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unidades de medida:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Unidad - Unid
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Servicios Profesionales - Sp
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">1 por metro - 1/m
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Alquiler de uso comercial - Alc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Alquiler de uso habitacional - Al
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Ampere - A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">ampere por metro - A/m
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">ampere por metro cuadrado - A/m²
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Becquerel - Bq
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">bel - B
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Candela - cd
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">candela por metro cuadrado - cd/m²
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">centímetro - cm
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Comisiones - Cm
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">coulomb - C
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">coulomb por kilogramo - C/kg
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">coulomb por metro cuadrado - C/m²
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">coulomb por metro cúbico - C/m³
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">día - d
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">electronvolt - eV
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">estereorradión - sr
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">farad - F
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">farad por metro - F/m
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Galán - Gal
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">grado - deg
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">grado Celsius - C
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Gramo - g
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">gray - Gy
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">gray por segundo - Gy/s
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">henry - H
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">henry por metro - H/m
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">hertz - Hz
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">hora - h
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Intereses - I
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Joule - J
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">joule por kelvin - J/K
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">joule por kilogramo - J/kg
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">joule por metro cúbico - J/m³
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">joule por mol - J/mol
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">katal - kat
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">katal por metro cúbico - kat/m³
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Kelvin - K
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Kilogramo - kg
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">kilogramo por metro cúbico - kg/m³
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Kilometro - Km
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">kilovatios - Kw
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">litro - L
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">lumen - lm
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">lux - lx
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Metro - m
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">metro cuadrado - m²
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">metro cúbico - m³
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">metro por segundo - m/s
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">mililitro - mL
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Milímetro - mm
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">minuto - min
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Mol - mol
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">mol por metro cúbico - mol/m³
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">neper - Np
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">newton - N
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">newton por metro - N/m
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Onzas - Oz
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Otro tipo de servicio - Os
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">pascal - Pa
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">pascal segundo - Pa s
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">pulgada - ln
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">radión - rad
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">radión por segundo - rad/s
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Se debe indicar la descripción de la medida a utilizar - Otros
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">segundo - s
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Servicios personales - Spe
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Servicios técnicos - St
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">siemens - S
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">sievert - Sv
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">tesla - T
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">tonelada - t
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">unidad astronómica - ua
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">unidad de masa atómica unificada - u
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">uno (indice de refracción) - 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">volt - V
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">volt por metro - V/m
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">Watt - W
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">watt por estereorradión - W/sr
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">watt por metro cuadrado - W/m²
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">watt por metro kevin - W/(mxK)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
+          </rPr>
+          <t xml:space="preserve">weber - Wb
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{113E9FA5-BE92-1D49-B526-F17CEC02F5F4}">
       <text>
         <r>
           <rPr>
@@ -1687,7 +1800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="1" shapeId="0" xr:uid="{87040AA1-A5AB-B347-832B-C2F6DF52CF29}">
+    <comment ref="X2" authorId="1" shapeId="0" xr:uid="{87040AA1-A5AB-B347-832B-C2F6DF52CF29}">
       <text>
         <r>
           <rPr>
@@ -3627,7 +3740,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{85F316E1-4EB4-AE4F-B3E9-92794A3C4B59}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{85F316E1-4EB4-AE4F-B3E9-92794A3C4B59}">
       <text>
         <r>
           <rPr>
@@ -3690,7 +3803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="1" shapeId="0" xr:uid="{D36217BF-BE60-014C-B578-179FD01A9ECB}">
+    <comment ref="AB2" authorId="1" shapeId="0" xr:uid="{D36217BF-BE60-014C-B578-179FD01A9ECB}">
       <text>
         <r>
           <rPr>
@@ -3758,7 +3871,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>ConsecutivoComprobante</t>
   </si>
@@ -3995,6 +4108,18 @@
   </si>
   <si>
     <t>ClaveFactura</t>
+  </si>
+  <si>
+    <t>CedulaEmpresa</t>
+  </si>
+  <si>
+    <t>Ingrese la cédula de su empresa o persona física en todas las columnas</t>
+  </si>
+  <si>
+    <t>310270XXXX</t>
+  </si>
+  <si>
+    <t>50624081900310167175100100001010000000267180706096</t>
   </si>
 </sst>
 </file>
@@ -4150,7 +4275,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4245,9 +4377,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -4264,43 +4393,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:AA4" headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24">
-  <autoFilter ref="A3:AA4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:Z4">
-    <sortCondition ref="C3:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:AB4" headerRowDxfId="27" dataDxfId="26" totalsRowDxfId="25">
+  <autoFilter ref="A3:AB4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AA4">
+    <sortCondition ref="D3:D4"/>
   </sortState>
-  <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TipoDocumento" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{9A6B3D5D-80B4-412F-8AAF-DDF5A95B8456}" name="ClaveFactura"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ConsecutivoComprobante" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Moneda" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TipoCambio" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FechaEmision" dataDxfId="19"/>
+  <tableColumns count="28">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CedulaEmpresa" dataDxfId="1"/>
+    <tableColumn id="28" xr3:uid="{60F9662E-6641-46DB-825D-4D1E03ED9305}" name="TipoDocumento"/>
+    <tableColumn id="17" xr3:uid="{9A6B3D5D-80B4-412F-8AAF-DDF5A95B8456}" name="ClaveFactura" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ConsecutivoComprobante" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Moneda" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TipoCambio" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FechaEmision" dataDxfId="21"/>
     <tableColumn id="26" xr3:uid="{BC57BDDF-3739-4B7D-AFAD-41175DE60537}" name="CodigoCliente"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NombreCliente" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TipoIdentificacion" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IdentificacionReceptor" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="NombreCliente" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TipoIdentificacion" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="IdentificacionReceptor" dataDxfId="18"/>
     <tableColumn id="14" xr3:uid="{9EE5C575-439A-401D-844A-0CF2ADD0E6CE}" name="CorreoReceptor"/>
     <tableColumn id="25" xr3:uid="{416EB538-A7AD-494E-B673-8B653787523A}" name="CondicionVenta"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="MetodoPago" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NumeroLinea" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="DetalleProducto" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CodigoProducto" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cantidad" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="UnidadMedicion" dataDxfId="10"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="PrecioUnitario" dataDxfId="9"/>
-    <tableColumn id="27" xr3:uid="{F2DD17B1-2A7F-44F4-9597-E795BCF624ED}" name="SubtotalLinea" dataDxfId="8">
-      <calculatedColumnFormula>Q4*S4</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="MetodoPago" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NumeroLinea" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="DetalleProducto" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CodigoProducto" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cantidad" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="UnidadMedicion" dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="PrecioUnitario" dataDxfId="11"/>
+    <tableColumn id="27" xr3:uid="{F2DD17B1-2A7F-44F4-9597-E795BCF624ED}" name="SubtotalLinea" dataDxfId="10">
+      <calculatedColumnFormula>R4*T4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MontoDescuento" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="CodigoIVAEtax" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{1EC5F6F2-FEE3-C141-B60F-1906E2188F5B}" name="CategoriaDeclaracion" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="MontoIVA" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TotalLinea" dataDxfId="3">
-      <calculatedColumnFormula>T4-U4+X4</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="MontoDescuento" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="CodigoIVAEtax" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{1EC5F6F2-FEE3-C141-B60F-1906E2188F5B}" name="CategoriaDeclaracion" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="MontoIVA" dataDxfId="6"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TotalLinea" dataDxfId="5">
+      <calculatedColumnFormula>U4-V4+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="TotalDocumento" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F89F5289-1050-F846-8BB8-93D35EA81D68}" name="ActividadComercial" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="TotalDocumento" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F89F5289-1050-F846-8BB8-93D35EA81D68}" name="ActividadComercial" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4603,38 +4733,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="7" width="15.77734375" customWidth="1"/>
-    <col min="8" max="8" width="20.77734375" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="10" max="11" width="20.77734375" customWidth="1"/>
-    <col min="12" max="19" width="15.77734375" customWidth="1"/>
-    <col min="20" max="20" width="25.77734375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="15.77734375" customWidth="1"/>
-    <col min="23" max="23" width="25.77734375" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" customWidth="1"/>
-    <col min="25" max="25" width="25.77734375" customWidth="1"/>
-    <col min="26" max="26" width="15.77734375" customWidth="1"/>
-    <col min="27" max="27" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+    <col min="7" max="8" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" customWidth="1"/>
+    <col min="11" max="12" width="20.77734375" customWidth="1"/>
+    <col min="13" max="20" width="15.77734375" customWidth="1"/>
+    <col min="21" max="21" width="25.77734375" style="1" customWidth="1"/>
+    <col min="22" max="23" width="15.77734375" customWidth="1"/>
+    <col min="24" max="24" width="25.77734375" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" customWidth="1"/>
+    <col min="26" max="26" width="25.77734375" customWidth="1"/>
+    <col min="27" max="27" width="15.77734375" customWidth="1"/>
+    <col min="28" max="28" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
@@ -4658,209 +4789,216 @@
       <c r="X1" s="17"/>
       <c r="Y1" s="17"/>
       <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
     </row>
-    <row r="2" spans="1:27" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="S2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>5.0624081900310098E+49</v>
-      </c>
       <c r="C4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4" s="8">
+      <c r="K4" s="8">
         <v>114170404</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="L4" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -4868,74 +5006,77 @@
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
         <v>24</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>25</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>48</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>1000</v>
       </c>
-      <c r="T4" s="1">
-        <f>Q4*S4</f>
+      <c r="U4" s="1">
+        <f>R4*T4</f>
         <v>1000</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>15</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>130</v>
       </c>
-      <c r="Y4" s="1">
-        <f>T4-U4+X4</f>
+      <c r="Z4" s="1">
+        <f>U4-V4+Y4</f>
         <v>1130</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>1130</v>
       </c>
-      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:Z1"/>
+    <mergeCell ref="A1:AA1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B4" xr:uid="{AC2F3921-FC38-9548-AC79-E72BE78E27E2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{AC2F3921-FC38-9548-AC79-E72BE78E27E2}">
       <formula1>"1, 2, 3, 4, 5, 6, 7, 8, 99"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4" xr:uid="{5A0A31C5-ACF9-4248-8C93-C275B189E2B8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{5A0A31C5-ACF9-4248-8C93-C275B189E2B8}">
       <formula1>"CRC, USD, EUR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4" xr:uid="{F6F97C31-42F3-F741-B38C-A1CF2550E246}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4" xr:uid="{F6F97C31-42F3-F741-B38C-A1CF2550E246}">
       <formula1>"1, 2, 3, 4, 5, 6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4" xr:uid="{A92A3769-41C2-0D49-8A4C-9157B560713C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4" xr:uid="{A92A3769-41C2-0D49-8A4C-9157B560713C}">
       <formula1>"1, 2, 3, 4, 5, 6, 99"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M4" xr:uid="{C57433FB-8CD1-5B4B-AF9A-CBC8E58F71F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4" xr:uid="{C57433FB-8CD1-5B4B-AF9A-CBC8E58F71F0}">
       <formula1>"1, 2, 3, 4, 5, 99"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{FDAD6757-4301-41CC-A48A-D6BB3898384E}"/>
+    <hyperlink ref="L4" r:id="rId1" xr:uid="{FDAD6757-4301-41CC-A48A-D6BB3898384E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="C4" numberStoredAsText="1"/>
+    <ignoredError sqref="D4" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId3"/>
   <tableParts count="1">

</xml_diff>